<commit_message>
Updated cost_clouds.csv file in input_samples directory - this version includes all ALPHA classes and years thru 2050.
</commit_message>
<xml_diff>
--- a/alpha_package_costs/alpha_package_costs_inputs/alpha_package_costs_module_inputs.xlsx
+++ b/alpha_package_costs/alpha_package_costs_inputs/alpha_package_costs_module_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\Documents\GitHub\EPA_OMEGA_Model\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\Documents\GitHub\EPA_OMEGA_Model\alpha_package_costs\alpha_package_costs_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C170D0-4E83-445F-90EE-6C2487EE4297}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DB6E17-5E9F-448A-94BF-655E41BE26BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="719" activeTab="11" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="719" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs_code" sheetId="15" r:id="rId1"/>
@@ -53,7 +53,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1916,8 +1918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF58B9CD-C45C-4464-97D6-845ECC18E560}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1946,7 +1948,7 @@
         <v>317</v>
       </c>
       <c r="B3" s="1">
-        <v>2035</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -4300,7 +4302,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3B69F5C-798B-4A10-94D8-33D9607CBCCB}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
alpha_package_costs_module.py now reads input_samples standards files to calc BEV targets. What input_samples file to read is controlled via the alpha_package_costs_module_inputs.xlsx file. New cost_clouds.csv file calculates BEV CO2/mile values using ghg_standards-flat.csv rather than footprints.
</commit_message>
<xml_diff>
--- a/alpha_package_costs/alpha_package_costs_inputs/alpha_package_costs_module_inputs.xlsx
+++ b/alpha_package_costs/alpha_package_costs_inputs/alpha_package_costs_module_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\Documents\GitHub\EPA_OMEGA_Model\alpha_package_costs\alpha_package_costs_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DB6E17-5E9F-448A-94BF-655E41BE26BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1CC8AE-5FDE-4873-8D88-1E0F666649BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="719" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
   </bookViews>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="338">
   <si>
     <t>SOHC</t>
   </si>
@@ -1105,6 +1105,15 @@
   </si>
   <si>
     <t>dollar/kWh_20WR</t>
+  </si>
+  <si>
+    <t>ghg_standards</t>
+  </si>
+  <si>
+    <t>flat</t>
+  </si>
+  <si>
+    <t>NO LONGER USED</t>
   </si>
 </sst>
 </file>
@@ -1118,7 +1127,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1261,6 +1270,14 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1399,7 +1416,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1472,6 +1489,7 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="34">
     <cellStyle name="Accent1 2" xfId="20" xr:uid="{D9FD632B-EF7F-49B6-8440-0774D2DADADB}"/>
@@ -1916,10 +1934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF58B9CD-C45C-4464-97D6-845ECC18E560}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1989,6 +2007,14 @@
       </c>
       <c r="B8" s="1">
         <v>2019</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>335</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -6919,9 +6945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82E34BFD-9265-45F1-BE2F-2D62A03D848B}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6929,6 +6953,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="44" t="s">
+        <v>337</v>
+      </c>
       <c r="B1" s="37" t="s">
         <v>307</v>
       </c>
@@ -8239,6 +8266,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Adding usepa_omega2_preproc/bea_tables where BEA price deflator tables can be stored. Adding price_deflators-aeo.csv input template. Changes to context_aeo.py to create an input_template of price_deflators. Changes to alpha_package_costs_module.py to make use of price_deflator input template rather than price deflators in the alpha_package_costs_module_inputs.xlsx file.
</commit_message>
<xml_diff>
--- a/alpha_package_costs/alpha_package_costs_inputs/alpha_package_costs_module_inputs.xlsx
+++ b/alpha_package_costs/alpha_package_costs_inputs/alpha_package_costs_module_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\Documents\GitHub\EPA_OMEGA_Model\alpha_package_costs\alpha_package_costs_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1CC8AE-5FDE-4873-8D88-1E0F666649BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C06F8A-0001-4A88-803A-2E38AB256BFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="719" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <sheet name="coefficients" sheetId="14" r:id="rId15"/>
     <sheet name="gdp_deflators" sheetId="16" r:id="rId16"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId17"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">aero!$A$1:$D$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">engine!$A$1:$AI$34</definedName>
@@ -42,7 +39,6 @@
     <definedName name="Null_6cyl_DMC">inputs_workbook!$B$3</definedName>
     <definedName name="Null_8cyl_DMC">inputs_workbook!$B$2</definedName>
     <definedName name="TRX10_">inputs_workbook!$B$5</definedName>
-    <definedName name="USD_2006">[1]Inputs!$B$17</definedName>
     <definedName name="workbook_dollar_basis">inputs_workbook!$B$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -1098,9 +1094,6 @@
     <t>bev_cost_intercept</t>
   </si>
   <si>
-    <t>analysis_year_dollars</t>
-  </si>
-  <si>
     <t>dollar/kWh_0WR</t>
   </si>
   <si>
@@ -1114,6 +1107,9 @@
   </si>
   <si>
     <t>NO LONGER USED</t>
+  </si>
+  <si>
+    <t>NOTE: these deflators are still used within this workbook even though the costs calculated within the workbook are subsequently adjusted using the Implicit Price Deflators (done in code) so there is a slight disconnect in the adjustments...but it's small.</t>
   </si>
 </sst>
 </file>
@@ -1540,69 +1536,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="ChangeLog"/>
-      <sheetName val="Inputs"/>
-      <sheetName val="CWC_VehType"/>
-      <sheetName val="TechList"/>
-      <sheetName val="LFs"/>
-      <sheetName val="ICMs"/>
-      <sheetName val="ICM_inputs"/>
-      <sheetName val="lfTable"/>
-      <sheetName val="ICM_o"/>
-      <sheetName val="ICM_w"/>
-      <sheetName val="et_dmc"/>
-      <sheetName val="wr_DMCcurves_FRM"/>
-      <sheetName val="wr_dmc"/>
-      <sheetName val="wr_DMCcurve_TAR"/>
-      <sheetName val="wr_dmc_TAR"/>
-      <sheetName val="wr_ICcurves"/>
-      <sheetName val="wr_ic_TAR"/>
-      <sheetName val="ev1_dmc_curves"/>
-      <sheetName val="ev1_dmc"/>
-      <sheetName val="ev2_dmc"/>
-      <sheetName val="T3"/>
-      <sheetName val="PriceDeflators"/>
-      <sheetName val="PU_Inputs"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="17">
-          <cell r="B17">
-            <v>1.175</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{046D2098-7ED5-4FD1-9252-DA736D36E254}" name="et_dmc" displayName="et_dmc" ref="A1:L62" totalsRowShown="0">
   <autoFilter ref="A1:L62" xr:uid="{FC23E305-CC0C-448F-8C6F-468416C8658D}">
@@ -1934,10 +1867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF58B9CD-C45C-4464-97D6-845ECC18E560}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2003,18 +1936,10 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>332</v>
-      </c>
-      <c r="B8" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+        <v>334</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -4408,10 +4333,10 @@
         <v>286</v>
       </c>
       <c r="R1" s="29" t="s">
+        <v>332</v>
+      </c>
+      <c r="S1" s="29" t="s">
         <v>333</v>
-      </c>
-      <c r="S1" s="29" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -6954,7 +6879,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B1" s="37" t="s">
         <v>307</v>
@@ -8272,10 +8197,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B101427-E0F5-4F9E-AF35-E5B072DEE02C}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B15"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8398,6 +8323,11 @@
       </c>
       <c r="B15" s="1">
         <v>112.348</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -8411,7 +8341,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8491,8 +8421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6B2318-32F9-4ECB-8F5A-79536977FADD}">
   <dimension ref="A1:AI31"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11859,7 +11789,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Adding AC costs to alpha_package_costs_module.py and alpha_package_costs_module_inputs.xlsx. Adding non-battery costs to alpha_package_costs_module_inputs.xlsx. cost_clouds.csv does not yet include these new costs.
</commit_message>
<xml_diff>
--- a/alpha_package_costs/alpha_package_costs_inputs/alpha_package_costs_module_inputs.xlsx
+++ b/alpha_package_costs/alpha_package_costs_inputs/alpha_package_costs_module_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\Documents\GitHub\EPA_OMEGA_Model\alpha_package_costs\alpha_package_costs_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6169C90A-4F60-4F25-9A82-6D58239630F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87026BE-454A-4D71-95FC-54F8C8D16B03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="719" firstSheet="1" activeTab="11" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="719" firstSheet="1" activeTab="10" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs_code" sheetId="15" r:id="rId1"/>
@@ -23,12 +23,13 @@
     <sheet name="aero" sheetId="6" r:id="rId8"/>
     <sheet name="nonaero" sheetId="9" r:id="rId9"/>
     <sheet name="deac" sheetId="10" r:id="rId10"/>
-    <sheet name="et_dmc" sheetId="7" r:id="rId11"/>
-    <sheet name="bev" sheetId="11" r:id="rId12"/>
-    <sheet name="bev_curves_data" sheetId="13" r:id="rId13"/>
-    <sheet name="upstream" sheetId="12" r:id="rId14"/>
-    <sheet name="coefficients" sheetId="14" r:id="rId15"/>
-    <sheet name="gdp_deflators" sheetId="16" r:id="rId16"/>
+    <sheet name="ac" sheetId="17" r:id="rId11"/>
+    <sheet name="et_dmc" sheetId="7" r:id="rId12"/>
+    <sheet name="bev" sheetId="11" r:id="rId13"/>
+    <sheet name="bev_curves_data" sheetId="13" r:id="rId14"/>
+    <sheet name="upstream" sheetId="12" r:id="rId15"/>
+    <sheet name="coefficients" sheetId="14" r:id="rId16"/>
+    <sheet name="gdp_deflators" sheetId="16" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">aero!$A$1:$D$3</definedName>
@@ -96,7 +97,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -118,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="345">
   <si>
     <t>SOHC</t>
   </si>
@@ -1144,6 +1145,15 @@
   </si>
   <si>
     <t>kWh; BATTERY_SUMMARY_BP4_NMC622_BEV250-350_v1.xlsx; BEV300, 450k</t>
+  </si>
+  <si>
+    <t>deletes</t>
+  </si>
+  <si>
+    <t>PEVHEVcosting_20180220.xlsx</t>
+  </si>
+  <si>
+    <t>ac_cost</t>
   </si>
 </sst>
 </file>
@@ -1452,7 +1462,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1527,6 +1537,9 @@
     <xf numFmtId="166" fontId="19" fillId="0" borderId="3" xfId="33" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="3" xfId="33" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="34">
     <cellStyle name="Accent1 2" xfId="20" xr:uid="{D9FD632B-EF7F-49B6-8440-0774D2DADADB}"/>
@@ -2099,6 +2112,65 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A4F4307-4CCE-4E39-8D04-CE4F082A04BF}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="4">
+        <f>C2*Markup</f>
+        <v>134.168240089752</v>
+      </c>
+      <c r="C2" s="1">
+        <v>89.445493393168007</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="4">
+        <f>C3*Markup</f>
+        <v>134.168240089752</v>
+      </c>
+      <c r="C3" s="1">
+        <v>89.445493393168007</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2010</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1C16C4-514C-4855-AC00-5CBAF6F7CA67}">
   <dimension ref="A1:L62"/>
   <sheetViews>
@@ -4290,11 +4362,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3B69F5C-798B-4A10-94D8-33D9607CBCCB}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -4405,20 +4477,20 @@
         <v>3281</v>
       </c>
       <c r="H2" s="45" cm="1">
-        <f t="array" ref="H2">INDEX(bev_curves_data!$M$37:$R$37,,MATCH($D2,bev_curves_data!$M$31:$R$31,0))</f>
+        <f t="array" ref="H2">INDEX(bev_curves_data!$M$47:$R$47,,MATCH($D2,bev_curves_data!$M$31:$R$31,0))</f>
         <v>-12.125242548355066</v>
       </c>
       <c r="I2" s="45" cm="1">
-        <f t="array" ref="I2">INDEX(bev_curves_data!$M$38:$R$38,,MATCH($D2,bev_curves_data!$M$31:$R$31,0))</f>
+        <f t="array" ref="I2">INDEX(bev_curves_data!$M$48:$R$48,,MATCH($D2,bev_curves_data!$M$31:$R$31,0))</f>
         <v>60.602629028559839</v>
       </c>
       <c r="J2" s="45" cm="1">
-        <f t="array" ref="J2">INDEX(bev_curves_data!$D$37:$I$37,,MATCH($D2,bev_curves_data!$D$31:$I$31,0))</f>
-        <v>-1245.8248078720785</v>
+        <f t="array" ref="J2">INDEX(bev_curves_data!$D$47:$I$47,,MATCH($D2,bev_curves_data!$D$31:$I$31,0))</f>
+        <v>-1190.4096392393747</v>
       </c>
       <c r="K2" s="45" cm="1">
-        <f t="array" ref="K2">INDEX(bev_curves_data!$D$38:$I$38,,MATCH($D2,bev_curves_data!$D$31:$I$31,0))</f>
-        <v>6885.1698170583295</v>
+        <f t="array" ref="K2">INDEX(bev_curves_data!$D$48:$I$48,,MATCH($D2,bev_curves_data!$D$31:$I$31,0))</f>
+        <v>9759.2455429171187</v>
       </c>
       <c r="L2" s="9">
         <v>2019</v>
@@ -4441,11 +4513,11 @@
       </c>
       <c r="R2" s="22">
         <f>K2/I2</f>
-        <v>113.61173479476602</v>
+        <v>161.03666952002919</v>
       </c>
       <c r="S2" s="22">
         <f>(J2*0.2+K2)/(H2*0.2+I2)</f>
-        <v>114.06464133257255</v>
+        <v>163.65691955817854</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4473,20 +4545,20 @@
         <v>3510</v>
       </c>
       <c r="H3" s="45" cm="1">
-        <f t="array" ref="H3">INDEX(bev_curves_data!$M$37:$R$37,,MATCH($D3,bev_curves_data!$M$31:$R$31,0))</f>
+        <f t="array" ref="H3">INDEX(bev_curves_data!$M$47:$R$47,,MATCH($D3,bev_curves_data!$M$31:$R$31,0))</f>
         <v>-16.97957801938189</v>
       </c>
       <c r="I3" s="45" cm="1">
-        <f t="array" ref="I3">INDEX(bev_curves_data!$M$38:$R$38,,MATCH($D3,bev_curves_data!$M$31:$R$31,0))</f>
+        <f t="array" ref="I3">INDEX(bev_curves_data!$M$48:$R$48,,MATCH($D3,bev_curves_data!$M$31:$R$31,0))</f>
         <v>66.831081073163773</v>
       </c>
       <c r="J3" s="45" cm="1">
-        <f t="array" ref="J3">INDEX(bev_curves_data!$D$37:$I$37,,MATCH($D3,bev_curves_data!$D$31:$I$31,0))</f>
-        <v>-1525.0172230698106</v>
+        <f t="array" ref="J3">INDEX(bev_curves_data!$D$47:$I$47,,MATCH($D3,bev_curves_data!$D$31:$I$31,0))</f>
+        <v>-1461.1214396077178</v>
       </c>
       <c r="K3" s="45" cm="1">
-        <f t="array" ref="K3">INDEX(bev_curves_data!$D$38:$I$38,,MATCH($D3,bev_curves_data!$D$31:$I$31,0))</f>
-        <v>7484.7761906287496</v>
+        <f t="array" ref="K3">INDEX(bev_curves_data!$D$48:$I$48,,MATCH($D3,bev_curves_data!$D$31:$I$31,0))</f>
+        <v>11225.908358130564</v>
       </c>
       <c r="L3" s="9">
         <v>2019</v>
@@ -4509,11 +4581,11 @@
       </c>
       <c r="R3" s="22">
         <f t="shared" ref="R3:R7" si="2">K3/I3</f>
-        <v>111.99543790762176</v>
+        <v>167.97436429078448</v>
       </c>
       <c r="S3" s="22">
         <f t="shared" ref="S3:S7" si="3">(J3*0.2+K3)/(H3*0.2+I3)</f>
-        <v>113.18284886465578</v>
+        <v>172.3599834464473</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4541,20 +4613,20 @@
         <v>3838</v>
       </c>
       <c r="H4" s="45" cm="1">
-        <f t="array" ref="H4">INDEX(bev_curves_data!$M$37:$R$37,,MATCH($D4,bev_curves_data!$M$31:$R$31,0))</f>
+        <f t="array" ref="H4">INDEX(bev_curves_data!$M$47:$R$47,,MATCH($D4,bev_curves_data!$M$31:$R$31,0))</f>
         <v>-20.472123941098509</v>
       </c>
       <c r="I4" s="45" cm="1">
-        <f t="array" ref="I4">INDEX(bev_curves_data!$M$38:$R$38,,MATCH($D4,bev_curves_data!$M$31:$R$31,0))</f>
+        <f t="array" ref="I4">INDEX(bev_curves_data!$M$48:$R$48,,MATCH($D4,bev_curves_data!$M$31:$R$31,0))</f>
         <v>70.839108273020074</v>
       </c>
       <c r="J4" s="45" cm="1">
-        <f t="array" ref="J4">INDEX(bev_curves_data!$D$37:$I$37,,MATCH($D4,bev_curves_data!$D$31:$I$31,0))</f>
-        <v>-1973.0040011117987</v>
+        <f t="array" ref="J4">INDEX(bev_curves_data!$D$47:$I$47,,MATCH($D4,bev_curves_data!$D$31:$I$31,0))</f>
+        <v>-1894.7707841858044</v>
       </c>
       <c r="K4" s="45" cm="1">
-        <f t="array" ref="K4">INDEX(bev_curves_data!$D$38:$I$38,,MATCH($D4,bev_curves_data!$D$31:$I$31,0))</f>
-        <v>7862.9862953498514</v>
+        <f t="array" ref="K4">INDEX(bev_curves_data!$D$48:$I$48,,MATCH($D4,bev_curves_data!$D$31:$I$31,0))</f>
+        <v>12396.838036451736</v>
       </c>
       <c r="L4" s="9">
         <v>2019</v>
@@ -4577,11 +4649,11 @@
       </c>
       <c r="R4" s="22">
         <f t="shared" si="2"/>
-        <v>110.99781585399437</v>
+        <v>174.99991655277825</v>
       </c>
       <c r="S4" s="22">
         <f t="shared" si="3"/>
-        <v>111.89483723940725</v>
+        <v>180.05754544257272</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4609,20 +4681,20 @@
         <v>4294</v>
       </c>
       <c r="H5" s="45" cm="1">
-        <f t="array" ref="H5">INDEX(bev_curves_data!$M$37:$R$37,,MATCH($D5,bev_curves_data!$M$31:$R$31,0))</f>
+        <f t="array" ref="H5">INDEX(bev_curves_data!$M$47:$R$47,,MATCH($D5,bev_curves_data!$M$31:$R$31,0))</f>
         <v>-25.594561016888299</v>
       </c>
       <c r="I5" s="45" cm="1">
-        <f t="array" ref="I5">INDEX(bev_curves_data!$M$38:$R$38,,MATCH($D5,bev_curves_data!$M$31:$R$31,0))</f>
+        <f t="array" ref="I5">INDEX(bev_curves_data!$M$48:$R$48,,MATCH($D5,bev_curves_data!$M$31:$R$31,0))</f>
         <v>76.618087250037277</v>
       </c>
       <c r="J5" s="45" cm="1">
-        <f t="array" ref="J5">INDEX(bev_curves_data!$D$37:$I$37,,MATCH($D5,bev_curves_data!$D$31:$I$31,0))</f>
-        <v>-3766.3207185782558</v>
+        <f t="array" ref="J5">INDEX(bev_curves_data!$D$47:$I$47,,MATCH($D5,bev_curves_data!$D$31:$I$31,0))</f>
+        <v>-3675.0674067380364</v>
       </c>
       <c r="K5" s="45" cm="1">
-        <f t="array" ref="K5">INDEX(bev_curves_data!$D$38:$I$38,,MATCH($D5,bev_curves_data!$D$31:$I$31,0))</f>
-        <v>8548.1465381185244</v>
+        <f t="array" ref="K5">INDEX(bev_curves_data!$D$48:$I$48,,MATCH($D5,bev_curves_data!$D$31:$I$31,0))</f>
+        <v>13948.015781500824</v>
       </c>
       <c r="L5" s="9">
         <v>2019</v>
@@ -4645,11 +4717,11 @@
       </c>
       <c r="R5" s="22">
         <f t="shared" si="2"/>
-        <v>111.56825816105668</v>
+        <v>182.04599308231931</v>
       </c>
       <c r="S5" s="22">
         <f t="shared" si="3"/>
-        <v>109.02059204621612</v>
+        <v>184.79936714697126</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4677,20 +4749,20 @@
         <v>4454</v>
       </c>
       <c r="H6" s="45" cm="1">
-        <f t="array" ref="H6">INDEX(bev_curves_data!$M$37:$R$37,,MATCH($D6,bev_curves_data!$M$31:$R$31,0))</f>
+        <f t="array" ref="H6">INDEX(bev_curves_data!$M$47:$R$47,,MATCH($D6,bev_curves_data!$M$31:$R$31,0))</f>
         <v>-30.741258993748659</v>
       </c>
       <c r="I6" s="45" cm="1">
-        <f t="array" ref="I6">INDEX(bev_curves_data!$M$38:$R$38,,MATCH($D6,bev_curves_data!$M$31:$R$31,0))</f>
+        <f t="array" ref="I6">INDEX(bev_curves_data!$M$48:$R$48,,MATCH($D6,bev_curves_data!$M$31:$R$31,0))</f>
         <v>92.23566087802449</v>
       </c>
       <c r="J6" s="45" cm="1">
-        <f t="array" ref="J6">INDEX(bev_curves_data!$D$37:$I$37,,MATCH($D6,bev_curves_data!$D$31:$I$31,0))</f>
-        <v>-2437.9820613806437</v>
+        <f t="array" ref="J6">INDEX(bev_curves_data!$D$47:$I$47,,MATCH($D6,bev_curves_data!$D$31:$I$31,0))</f>
+        <v>-2323.1666671980433</v>
       </c>
       <c r="K6" s="45" cm="1">
-        <f t="array" ref="K6">INDEX(bev_curves_data!$D$38:$I$38,,MATCH($D6,bev_curves_data!$D$31:$I$31,0))</f>
-        <v>9817.8288936903355</v>
+        <f t="array" ref="K6">INDEX(bev_curves_data!$D$48:$I$48,,MATCH($D6,bev_curves_data!$D$31:$I$31,0))</f>
+        <v>15645.982809469857</v>
       </c>
       <c r="L6" s="9">
         <v>2019</v>
@@ -4713,11 +4785,11 @@
       </c>
       <c r="R6" s="22">
         <f t="shared" si="2"/>
-        <v>106.44287469977321</v>
+        <v>169.63051666275396</v>
       </c>
       <c r="S6" s="22">
         <f t="shared" si="3"/>
-        <v>108.38091866398645</v>
+        <v>176.34808200639765</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4745,20 +4817,20 @@
         <v>5310</v>
       </c>
       <c r="H7" s="45" cm="1">
-        <f t="array" ref="H7">INDEX(bev_curves_data!$M$37:$R$37,,MATCH($D7,bev_curves_data!$M$31:$R$31,0))</f>
+        <f t="array" ref="H7">INDEX(bev_curves_data!$M$47:$R$47,,MATCH($D7,bev_curves_data!$M$31:$R$31,0))</f>
         <v>-34.041987144201435</v>
       </c>
       <c r="I7" s="45" cm="1">
-        <f t="array" ref="I7">INDEX(bev_curves_data!$M$38:$R$38,,MATCH($D7,bev_curves_data!$M$31:$R$31,0))</f>
+        <f t="array" ref="I7">INDEX(bev_curves_data!$M$48:$R$48,,MATCH($D7,bev_curves_data!$M$31:$R$31,0))</f>
         <v>100.81700213237262</v>
       </c>
       <c r="J7" s="45" cm="1">
-        <f t="array" ref="J7">INDEX(bev_curves_data!$D$37:$I$37,,MATCH($D7,bev_curves_data!$D$31:$I$31,0))</f>
-        <v>-4418.2971385683086</v>
+        <f t="array" ref="J7">INDEX(bev_curves_data!$D$47:$I$47,,MATCH($D7,bev_curves_data!$D$31:$I$31,0))</f>
+        <v>-4248.4001872690988</v>
       </c>
       <c r="K7" s="45" cm="1">
-        <f t="array" ref="K7">INDEX(bev_curves_data!$D$38:$I$38,,MATCH($D7,bev_curves_data!$D$31:$I$31,0))</f>
-        <v>10756.237698411596</v>
+        <f t="array" ref="K7">INDEX(bev_curves_data!$D$48:$I$48,,MATCH($D7,bev_curves_data!$D$31:$I$31,0))</f>
+        <v>16756.64388209338</v>
       </c>
       <c r="L7" s="9">
         <v>2019</v>
@@ -4781,11 +4853,11 @@
       </c>
       <c r="R7" s="22">
         <f t="shared" si="2"/>
-        <v>106.69071159533853</v>
+        <v>166.20851173586698</v>
       </c>
       <c r="S7" s="22">
         <f t="shared" si="3"/>
-        <v>105.01781514396816</v>
+        <v>169.20753046813238</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
@@ -5013,12 +5085,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F787BE-7CDC-4D53-B66A-224AC26D0702}">
-  <dimension ref="A1:V38"/>
+  <dimension ref="A1:V51"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="M37" sqref="M37:R38"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6324,43 +6396,43 @@
       <c r="C32" s="17">
         <v>0</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="1">
         <v>6986.7903156711445</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="1">
         <v>7558.3654190903089</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="1">
         <v>7952.5935020381576</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="1">
         <v>8664.7752526713557</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="1">
         <v>9970.6230202013594</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="1">
         <v>10985.367179559473</v>
       </c>
       <c r="L32" s="34">
         <v>0</v>
       </c>
-      <c r="M32">
+      <c r="M32" s="1">
         <v>61.302528341787323</v>
       </c>
-      <c r="N32">
+      <c r="N32" s="1">
         <v>67.775194005951221</v>
       </c>
-      <c r="O32">
+      <c r="O32" s="1">
         <v>71.970961080436737</v>
       </c>
-      <c r="P32">
+      <c r="P32" s="1">
         <v>77.968544352784122</v>
       </c>
-      <c r="Q32">
+      <c r="Q32" s="1">
         <v>94.169058891645932</v>
       </c>
-      <c r="R32">
+      <c r="R32" s="1">
         <v>103.07282791177303</v>
       </c>
     </row>
@@ -6368,43 +6440,43 @@
       <c r="C33" s="17">
         <v>0.02</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="1">
         <v>6843.108841416396</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="1">
         <v>7477.0984324135088</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="1">
         <v>7857.531065717506</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="1">
         <v>8545.1633937679126</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="1">
         <v>9790.3593283403497</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="1">
         <v>10763.31452153694</v>
       </c>
       <c r="L33" s="34">
         <v>0.02</v>
       </c>
-      <c r="M33">
+      <c r="M33" s="1">
         <v>60.537388583682542</v>
       </c>
-      <c r="N33">
+      <c r="N33" s="1">
         <v>66.753499830227014</v>
       </c>
-      <c r="O33">
+      <c r="O33" s="1">
         <v>70.770764666036172</v>
       </c>
-      <c r="P33">
+      <c r="P33" s="1">
         <v>76.497450849801709</v>
       </c>
-      <c r="Q33">
+      <c r="Q33" s="1">
         <v>91.881041688994586</v>
       </c>
-      <c r="R33">
+      <c r="R33" s="1">
         <v>100.2876054651894</v>
       </c>
     </row>
@@ -6412,43 +6484,43 @@
       <c r="C34" s="17">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="1">
         <v>6701.3020418562</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="1">
         <v>7285.3648671357159</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="1">
         <v>7608.4347912342137</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="1">
         <v>8091.7847200854958</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="1">
         <v>9455.0848118075046</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="1">
         <v>10095.794148411251</v>
       </c>
       <c r="L34" s="34">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="M34">
+      <c r="M34" s="1">
         <v>58.7946431968398</v>
       </c>
-      <c r="N34">
+      <c r="N34" s="1">
         <v>64.347306962647608</v>
       </c>
-      <c r="O34">
+      <c r="O34" s="1">
         <v>67.813730252868439</v>
       </c>
-      <c r="P34">
+      <c r="P34" s="1">
         <v>72.928726031037726</v>
       </c>
-      <c r="Q34">
+      <c r="Q34" s="1">
         <v>87.661940362931901</v>
       </c>
-      <c r="R34">
+      <c r="R34" s="1">
         <v>95.759495559138685</v>
       </c>
     </row>
@@ -6456,43 +6528,43 @@
       <c r="C35" s="17">
         <v>0.1</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="1">
         <v>6701.2450453822303</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="1">
         <v>7250.3091458590716</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="1">
         <v>7558.4830062005722</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="1">
         <v>8025.398856291893</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="1">
         <v>9454.9895820496076</v>
       </c>
-      <c r="I35">
+      <c r="I35" s="1">
         <v>10095.691124404575</v>
       </c>
       <c r="L35" s="34">
         <v>0.1</v>
       </c>
-      <c r="M35">
+      <c r="M35" s="1">
         <v>58.794471017049482</v>
       </c>
-      <c r="N35">
+      <c r="N35" s="1">
         <v>64.286161033067287</v>
       </c>
-      <c r="O35">
+      <c r="O35" s="1">
         <v>67.776673200479891</v>
       </c>
-      <c r="P35">
+      <c r="P35" s="1">
         <v>72.865669695086993</v>
       </c>
-      <c r="Q35">
+      <c r="Q35" s="1">
         <v>87.661525781087377</v>
       </c>
-      <c r="R35">
+      <c r="R35" s="1">
         <v>95.759001244663736</v>
       </c>
     </row>
@@ -6500,156 +6572,475 @@
       <c r="C36" s="17">
         <v>0.2</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="1">
         <v>6701.3020418562046</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="1">
         <v>7250.3612855325709</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="1">
         <v>7558.552531119647</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="1">
         <v>7925.9137839375526</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="1">
         <v>9455.0848118075101</v>
       </c>
-      <c r="I36">
+      <c r="I36" s="1">
         <v>10095.794148411251</v>
       </c>
       <c r="L36" s="34">
         <v>0.2</v>
       </c>
-      <c r="M36">
+      <c r="M36" s="1">
         <v>58.7946431968398</v>
       </c>
-      <c r="N36">
+      <c r="N36" s="1">
         <v>64.286310216269911</v>
       </c>
-      <c r="O36">
+      <c r="O36" s="1">
         <v>67.776923208545185</v>
       </c>
-      <c r="P36">
+      <c r="P36" s="1">
         <v>72.720193719804982</v>
       </c>
-      <c r="Q36">
+      <c r="Q36" s="1">
         <v>87.661940362931901</v>
       </c>
-      <c r="R36">
+      <c r="R36" s="1">
         <v>95.759495559138685</v>
       </c>
     </row>
-    <row r="37" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="C37" s="17" t="s">
+    <row r="37" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="34">
+        <v>0</v>
+      </c>
+      <c r="D37" s="34">
+        <f>($D$8*$C32+$E$8)+ABS(D$50)</f>
+        <v>2874.0757258587901</v>
+      </c>
+      <c r="E37" s="34">
+        <f>($D$9*$C32+$E$9)+ABS(E$50)</f>
+        <v>3741.1321675018125</v>
+      </c>
+      <c r="F37" s="34">
+        <f>($D$10*$C32+$E$10)+ABS(F$50)</f>
+        <v>4533.8517411018856</v>
+      </c>
+      <c r="G37" s="34">
+        <f>($D$11*$C32+$E$11)+ABS(G$50)</f>
+        <v>5399.8692433822989</v>
+      </c>
+      <c r="H37" s="34">
+        <f>($D$12*$C32+$E$12)+ABS(H$50)</f>
+        <v>5828.1539157795196</v>
+      </c>
+      <c r="I37" s="34">
+        <f>($D$13*$C32+$E$13)+ABS(I$50)</f>
+        <v>6000.4061836817873</v>
+      </c>
+    </row>
+    <row r="38" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="34">
+        <v>0.02</v>
+      </c>
+      <c r="D38" s="34">
+        <f t="shared" ref="D38:D41" si="21">($D$8*$C33+$E$8)+ABS(D$50)</f>
+        <v>2875.1840292314441</v>
+      </c>
+      <c r="E38" s="34">
+        <f t="shared" ref="E38:E41" si="22">($D$9*$C33+$E$9)+ABS(E$50)</f>
+        <v>3742.4100831710548</v>
+      </c>
+      <c r="F38" s="34">
+        <f t="shared" ref="F38:F41" si="23">($D$10*$C33+$E$10)+ABS(F$50)</f>
+        <v>4535.4164054404055</v>
+      </c>
+      <c r="G38" s="34">
+        <f t="shared" ref="G38:G41" si="24">($D$11*$C33+$E$11)+ABS(G$50)</f>
+        <v>5401.6943096191026</v>
+      </c>
+      <c r="H38" s="34">
+        <f t="shared" ref="H38:H41" si="25">($D$12*$C33+$E$12)+ABS(H$50)</f>
+        <v>5830.4502236631715</v>
+      </c>
+      <c r="I38" s="34">
+        <f t="shared" ref="I38:I41" si="26">($D$13*$C33+$E$13)+ABS(I$50)</f>
+        <v>6003.804122707772</v>
+      </c>
+    </row>
+    <row r="39" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="34">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D39" s="34">
+        <f t="shared" si="21"/>
+        <v>2878.2318635062425</v>
+      </c>
+      <c r="E39" s="34">
+        <f t="shared" si="22"/>
+        <v>3745.9243512614703</v>
+      </c>
+      <c r="F39" s="34">
+        <f t="shared" si="23"/>
+        <v>4539.7192323713352</v>
+      </c>
+      <c r="G39" s="34">
+        <f t="shared" si="24"/>
+        <v>5406.7132417703151</v>
+      </c>
+      <c r="H39" s="34">
+        <f t="shared" si="25"/>
+        <v>5836.7650703432146</v>
+      </c>
+      <c r="I39" s="34">
+        <f t="shared" si="26"/>
+        <v>6013.1484550292289</v>
+      </c>
+    </row>
+    <row r="40" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="34">
+        <v>0.1</v>
+      </c>
+      <c r="D40" s="34">
+        <f t="shared" si="21"/>
+        <v>2879.6172427220599</v>
+      </c>
+      <c r="E40" s="34">
+        <f t="shared" si="22"/>
+        <v>3747.5217458480224</v>
+      </c>
+      <c r="F40" s="34">
+        <f t="shared" si="23"/>
+        <v>4541.6750627944848</v>
+      </c>
+      <c r="G40" s="34">
+        <f t="shared" si="24"/>
+        <v>5408.9945745663208</v>
+      </c>
+      <c r="H40" s="34">
+        <f t="shared" si="25"/>
+        <v>5839.6354551977793</v>
+      </c>
+      <c r="I40" s="34">
+        <f t="shared" si="26"/>
+        <v>6017.3958788117088</v>
+      </c>
+    </row>
+    <row r="41" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="34">
+        <v>0.2</v>
+      </c>
+      <c r="D41" s="34">
+        <f t="shared" si="21"/>
+        <v>2885.1587595853298</v>
+      </c>
+      <c r="E41" s="34">
+        <f t="shared" si="22"/>
+        <v>3753.9113241942323</v>
+      </c>
+      <c r="F41" s="34">
+        <f t="shared" si="23"/>
+        <v>4549.498384487084</v>
+      </c>
+      <c r="G41" s="34">
+        <f t="shared" si="24"/>
+        <v>5418.1199057503427</v>
+      </c>
+      <c r="H41" s="34">
+        <f t="shared" si="25"/>
+        <v>5851.116994616038</v>
+      </c>
+      <c r="I41" s="34">
+        <f t="shared" si="26"/>
+        <v>6034.3855739416304</v>
+      </c>
+    </row>
+    <row r="42" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="34">
+        <v>0</v>
+      </c>
+      <c r="D42" s="34">
+        <f>SUM(D32,D37)</f>
+        <v>9860.8660415299346</v>
+      </c>
+      <c r="E42" s="34">
+        <f>SUM(E32,E37)</f>
+        <v>11299.497586592122</v>
+      </c>
+      <c r="F42" s="34">
+        <f t="shared" ref="F42:I42" si="27">SUM(F32,F37)</f>
+        <v>12486.445243140042</v>
+      </c>
+      <c r="G42" s="34">
+        <f t="shared" si="27"/>
+        <v>14064.644496053654</v>
+      </c>
+      <c r="H42" s="34">
+        <f t="shared" si="27"/>
+        <v>15798.776935980879</v>
+      </c>
+      <c r="I42" s="34">
+        <f t="shared" si="27"/>
+        <v>16985.77336324126</v>
+      </c>
+    </row>
+    <row r="43" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="34">
+        <v>0.02</v>
+      </c>
+      <c r="D43" s="34">
+        <f t="shared" ref="D43:E46" si="28">SUM(D33,D38)</f>
+        <v>9718.2928706478397</v>
+      </c>
+      <c r="E43" s="34">
+        <f>SUM(E33,E38)</f>
+        <v>11219.508515584563</v>
+      </c>
+      <c r="F43" s="34">
+        <f t="shared" ref="F43:I43" si="29">SUM(F33,F38)</f>
+        <v>12392.947471157911</v>
+      </c>
+      <c r="G43" s="34">
+        <f t="shared" si="29"/>
+        <v>13946.857703387015</v>
+      </c>
+      <c r="H43" s="34">
+        <f t="shared" si="29"/>
+        <v>15620.80955200352</v>
+      </c>
+      <c r="I43" s="34">
+        <f t="shared" si="29"/>
+        <v>16767.118644244714</v>
+      </c>
+    </row>
+    <row r="44" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="34">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D44" s="34">
+        <f t="shared" si="28"/>
+        <v>9579.533905362443</v>
+      </c>
+      <c r="E44" s="34">
+        <f t="shared" si="28"/>
+        <v>11031.289218397185</v>
+      </c>
+      <c r="F44" s="34">
+        <f t="shared" ref="F44:I44" si="30">SUM(F34,F39)</f>
+        <v>12148.154023605548</v>
+      </c>
+      <c r="G44" s="34">
+        <f t="shared" si="30"/>
+        <v>13498.49796185581</v>
+      </c>
+      <c r="H44" s="34">
+        <f t="shared" si="30"/>
+        <v>15291.84988215072</v>
+      </c>
+      <c r="I44" s="34">
+        <f t="shared" si="30"/>
+        <v>16108.942603440479</v>
+      </c>
+    </row>
+    <row r="45" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="34">
+        <v>0.1</v>
+      </c>
+      <c r="D45" s="34">
+        <f t="shared" si="28"/>
+        <v>9580.8622881042902</v>
+      </c>
+      <c r="E45" s="34">
+        <f t="shared" si="28"/>
+        <v>10997.830891707094</v>
+      </c>
+      <c r="F45" s="34">
+        <f t="shared" ref="F45:I45" si="31">SUM(F35,F40)</f>
+        <v>12100.158068995057</v>
+      </c>
+      <c r="G45" s="34">
+        <f t="shared" si="31"/>
+        <v>13434.393430858214</v>
+      </c>
+      <c r="H45" s="34">
+        <f t="shared" si="31"/>
+        <v>15294.625037247388</v>
+      </c>
+      <c r="I45" s="34">
+        <f t="shared" si="31"/>
+        <v>16113.087003216284</v>
+      </c>
+    </row>
+    <row r="46" spans="3:18" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="34">
+        <v>0.2</v>
+      </c>
+      <c r="D46" s="34">
+        <f t="shared" si="28"/>
+        <v>9586.4608014415353</v>
+      </c>
+      <c r="E46" s="34">
+        <f t="shared" si="28"/>
+        <v>11004.272609726802</v>
+      </c>
+      <c r="F46" s="34">
+        <f t="shared" ref="F46:I46" si="32">SUM(F36,F41)</f>
+        <v>12108.050915606731</v>
+      </c>
+      <c r="G46" s="34">
+        <f t="shared" si="32"/>
+        <v>13344.033689687894</v>
+      </c>
+      <c r="H46" s="34">
+        <f t="shared" si="32"/>
+        <v>15306.201806423549</v>
+      </c>
+      <c r="I46" s="34">
+        <f t="shared" si="32"/>
+        <v>16130.179722352881</v>
+      </c>
+    </row>
+    <row r="47" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C47" s="17" t="s">
         <v>338</v>
       </c>
-      <c r="D37" s="44">
-        <f>SLOPE( D$32:D$36,$C$32:$C$36)</f>
-        <v>-1245.8248078720785</v>
-      </c>
-      <c r="E37" s="44">
-        <f t="shared" ref="E37:I37" si="21">SLOPE( E$32:E$36,$C$32:$C$36)</f>
-        <v>-1525.0172230698106</v>
-      </c>
-      <c r="F37" s="44">
-        <f t="shared" si="21"/>
-        <v>-1973.0040011117987</v>
-      </c>
-      <c r="G37" s="44">
-        <f t="shared" si="21"/>
-        <v>-3766.3207185782558</v>
-      </c>
-      <c r="H37" s="44">
-        <f t="shared" si="21"/>
-        <v>-2437.9820613806437</v>
-      </c>
-      <c r="I37" s="44">
-        <f t="shared" si="21"/>
-        <v>-4418.2971385683086</v>
-      </c>
-      <c r="L37" s="34" t="s">
+      <c r="D47" s="44">
+        <f t="shared" ref="D47:I47" si="33">SLOPE( D$42:D$46,$C$42:$C$46)</f>
+        <v>-1190.4096392393747</v>
+      </c>
+      <c r="E47" s="44">
+        <f t="shared" si="33"/>
+        <v>-1461.1214396077178</v>
+      </c>
+      <c r="F47" s="44">
+        <f t="shared" si="33"/>
+        <v>-1894.7707841858044</v>
+      </c>
+      <c r="G47" s="44">
+        <f t="shared" si="33"/>
+        <v>-3675.0674067380364</v>
+      </c>
+      <c r="H47" s="44">
+        <f t="shared" si="33"/>
+        <v>-2323.1666671980433</v>
+      </c>
+      <c r="I47" s="44">
+        <f t="shared" si="33"/>
+        <v>-4248.4001872690988</v>
+      </c>
+      <c r="L47" s="34" t="s">
         <v>338</v>
       </c>
-      <c r="M37" s="44">
+      <c r="M47" s="44">
         <f>SLOPE( M$32:M$36,$L$32:$L$36)</f>
         <v>-12.125242548355066</v>
       </c>
-      <c r="N37" s="44">
-        <f t="shared" ref="N37:R37" si="22">SLOPE( N$32:N$36,$L$32:$L$36)</f>
+      <c r="N47" s="44">
+        <f t="shared" ref="N47:R47" si="34">SLOPE( N$32:N$36,$L$32:$L$36)</f>
         <v>-16.97957801938189</v>
       </c>
-      <c r="O37" s="44">
-        <f t="shared" si="22"/>
+      <c r="O47" s="44">
+        <f t="shared" si="34"/>
         <v>-20.472123941098509</v>
       </c>
-      <c r="P37" s="44">
-        <f t="shared" si="22"/>
+      <c r="P47" s="44">
+        <f t="shared" si="34"/>
         <v>-25.594561016888299</v>
       </c>
-      <c r="Q37" s="44">
-        <f t="shared" si="22"/>
+      <c r="Q47" s="44">
+        <f t="shared" si="34"/>
         <v>-30.741258993748659</v>
       </c>
-      <c r="R37" s="44">
-        <f t="shared" si="22"/>
+      <c r="R47" s="44">
+        <f t="shared" si="34"/>
         <v>-34.041987144201435</v>
       </c>
     </row>
-    <row r="38" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="C38" s="17" t="s">
+    <row r="48" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C48" s="17" t="s">
         <v>339</v>
       </c>
-      <c r="D38" s="44">
-        <f>INTERCEPT( D$32:D$36,$C$32:$C$36)</f>
-        <v>6885.1698170583295</v>
-      </c>
-      <c r="E38" s="44">
-        <f t="shared" ref="E38:I38" si="23">INTERCEPT( E$32:E$36,$C$32:$C$36)</f>
-        <v>7484.7761906287496</v>
-      </c>
-      <c r="F38" s="44">
-        <f t="shared" si="23"/>
-        <v>7862.9862953498514</v>
-      </c>
-      <c r="G38" s="44">
-        <f t="shared" si="23"/>
-        <v>8548.1465381185244</v>
-      </c>
-      <c r="H38" s="44">
-        <f t="shared" si="23"/>
-        <v>9817.8288936903355</v>
-      </c>
-      <c r="I38" s="44">
-        <f t="shared" si="23"/>
-        <v>10756.237698411596</v>
-      </c>
-      <c r="L38" s="34" t="s">
+      <c r="D48" s="44">
+        <f t="shared" ref="D48:I48" si="35">INTERCEPT( D$42:D$46,$C$42:$C$46)</f>
+        <v>9759.2455429171187</v>
+      </c>
+      <c r="E48" s="44">
+        <f t="shared" si="35"/>
+        <v>11225.908358130564</v>
+      </c>
+      <c r="F48" s="44">
+        <f t="shared" si="35"/>
+        <v>12396.838036451736</v>
+      </c>
+      <c r="G48" s="44">
+        <f t="shared" si="35"/>
+        <v>13948.015781500824</v>
+      </c>
+      <c r="H48" s="44">
+        <f t="shared" si="35"/>
+        <v>15645.982809469857</v>
+      </c>
+      <c r="I48" s="44">
+        <f t="shared" si="35"/>
+        <v>16756.64388209338</v>
+      </c>
+      <c r="L48" s="34" t="s">
         <v>339</v>
       </c>
-      <c r="M38" s="44">
+      <c r="M48" s="44">
         <f>INTERCEPT( M$32:M$36,$L$32:$L$36)</f>
         <v>60.602629028559839</v>
       </c>
-      <c r="N38" s="44">
-        <f t="shared" ref="N38:R38" si="24">INTERCEPT( N$32:N$36,$L$32:$L$36)</f>
+      <c r="N48" s="44">
+        <f t="shared" ref="N48:R48" si="36">INTERCEPT( N$32:N$36,$L$32:$L$36)</f>
         <v>66.831081073163773</v>
       </c>
-      <c r="O38" s="44">
-        <f t="shared" si="24"/>
+      <c r="O48" s="44">
+        <f t="shared" si="36"/>
         <v>70.839108273020074</v>
       </c>
-      <c r="P38" s="44">
-        <f t="shared" si="24"/>
+      <c r="P48" s="44">
+        <f t="shared" si="36"/>
         <v>76.618087250037277</v>
       </c>
-      <c r="Q38" s="44">
-        <f t="shared" si="24"/>
+      <c r="Q48" s="44">
+        <f t="shared" si="36"/>
         <v>92.23566087802449</v>
       </c>
-      <c r="R38" s="44">
-        <f t="shared" si="24"/>
+      <c r="R48" s="44">
+        <f t="shared" si="36"/>
         <v>100.81700213237262</v>
+      </c>
+    </row>
+    <row r="50" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C50" s="17" t="s">
+        <v>342</v>
+      </c>
+      <c r="D50" s="46">
+        <v>-3644.8139166666665</v>
+      </c>
+      <c r="E50" s="46">
+        <v>-4324.6949999999997</v>
+      </c>
+      <c r="F50" s="46">
+        <v>-4910.8609166666665</v>
+      </c>
+      <c r="G50" s="46">
+        <v>-5585.3516666666674</v>
+      </c>
+      <c r="H50" s="46">
+        <v>-5625.3516666666674</v>
+      </c>
+      <c r="I50" s="48">
+        <f>H50</f>
+        <v>-5625.3516666666674</v>
+      </c>
+    </row>
+    <row r="51" spans="3:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C51" s="47" t="s">
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -6659,7 +7050,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42C4D92A-6996-4221-BCA6-9F7B1FEA98B2}">
   <dimension ref="A1:E41"/>
   <sheetViews>
@@ -7287,7 +7678,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82E34BFD-9265-45F1-BE2F-2D62A03D848B}">
   <dimension ref="A1:M32"/>
   <sheetViews>
@@ -8616,7 +9007,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B101427-E0F5-4F9E-AF35-E5B072DEE02C}">
   <dimension ref="A1:B18"/>
   <sheetViews>
@@ -8842,8 +9233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6B2318-32F9-4ECB-8F5A-79536977FADD}">
   <dimension ref="A1:AI31"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12762,7 +13153,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated BEV sizing calcs using approach laid out by Mike S. and Ben E. Updated ALPHA run file for Bolt to cherry pick some packages for inclusion.
</commit_message>
<xml_diff>
--- a/alpha_package_costs/alpha_package_costs_inputs/alpha_package_costs_module_inputs.xlsx
+++ b/alpha_package_costs/alpha_package_costs_inputs/alpha_package_costs_module_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\Documents\GitHub\EPA_OMEGA_Model\alpha_package_costs\alpha_package_costs_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2A3BD7-F7A4-4D15-A31F-4DD3B03EFC3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544DDC08-F045-4A15-8AB6-69678B9CCCDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="826" firstSheet="2" activeTab="13" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
   </bookViews>
@@ -5112,7 +5112,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5228,7 +5228,7 @@
         <v>251</v>
       </c>
       <c r="B8" s="1">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>

</xml_diff>